<commit_message>
Reports upgraded... Version chanhed to 2.03.
</commit_message>
<xml_diff>
--- a/reports/daily_templ.xlsx
+++ b/reports/daily_templ.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t xml:space="preserve">Суточный отчет</t>
   </si>
@@ -34,6 +34,18 @@
     <t xml:space="preserve">Время</t>
   </si>
   <si>
+    <t xml:space="preserve">Темп., С </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Напр. ветра, град. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Скор. ветра, м/с </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Отн. влажность, % </t>
+  </si>
+  <si>
     <t xml:space="preserve">Концентрация, мг/м.куб. </t>
   </si>
   <si>
@@ -98,6 +110,18 @@
   </si>
   <si>
     <t xml:space="preserve">{d[i].values [i].pollution[i].time}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{d[i].values [i].pollution[i].valueTemp}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{d[i].values [i].pollution[i].valueDir}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{d[i].values [i].pollution[i].valueSpd}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{d[i].values [i].pollution[i].valueHum}</t>
   </si>
   <si>
     <t xml:space="preserve">{d[i].values [i].pollution[i].valueNO}</t>
@@ -170,7 +194,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -194,16 +218,8 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="12"/>
-      <color rgb="FF00000A"/>
+      <sz val="14"/>
       <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF00000A"/>
-      <name val="Liberation Serif;Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
     </font>
@@ -217,16 +233,29 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00000A"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF00000A"/>
       <name val="Liberation Serif;Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF00000A"/>
-      <name val="Liberation Serif;Times New Roman"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -237,7 +266,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -252,6 +281,13 @@
       <bottom style="hair"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -278,25 +314,33 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -315,18 +359,22 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -396,17 +444,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U13"/>
+  <dimension ref="A1:Y13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U15" activeCellId="0" sqref="U15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.85"/>
+  <sheetFormatPr defaultColWidth="8.19140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.2397959183673"/>
-    <col collapsed="false" hidden="false" max="21" min="2" style="0" width="11.7244897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.17857142857143"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="11.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="6" style="0" width="11.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -433,18 +480,22 @@
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -460,18 +511,30 @@
       <c r="S2" s="3"/>
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
+      <c r="C3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -487,173 +550,202 @@
       <c r="S3" s="4"/>
       <c r="T3" s="4"/>
       <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="21.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4"/>
-      <c r="B4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="5" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="O4" s="5" t="s">
+      <c r="O4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="P4" s="5" t="s">
+      <c r="P4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Q4" s="5" t="s">
+      <c r="Q4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="R4" s="5" t="s">
+      <c r="R4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="S4" s="5" t="s">
+      <c r="S4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="T4" s="5" t="s">
+      <c r="T4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="U4" s="5" t="s">
+      <c r="U4" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="V4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="W4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="X4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y4" s="7" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="7" t="s">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="B5" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="C5" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="D5" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="E5" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="F5" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="G5" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="H5" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="M5" s="7" t="s">
+      <c r="I5" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="N5" s="7" t="s">
+      <c r="J5" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="O5" s="7" t="s">
+      <c r="K5" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="P5" s="7" t="s">
+      <c r="L5" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="Q5" s="7" t="s">
+      <c r="M5" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="R5" s="7" t="s">
+      <c r="N5" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="S5" s="7" t="s">
+      <c r="O5" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="T5" s="7" t="s">
+      <c r="P5" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="U5" s="8" t="s">
+      <c r="Q5" s="11" t="s">
         <v>45</v>
       </c>
+      <c r="R5" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="S5" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="T5" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="U5" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="V5" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="W5" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="X5" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y5" s="11" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="9"/>
-      <c r="S6" s="9"/>
-      <c r="T6" s="9"/>
-      <c r="U6" s="9"/>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="12"/>
+      <c r="U6" s="12"/>
+      <c r="V6" s="12"/>
+      <c r="W6" s="12"/>
+      <c r="X6" s="12"/>
+      <c r="Y6" s="12"/>
     </row>
-    <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="9"/>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G13" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:U1"/>
-    <mergeCell ref="B2:U2"/>
+  <mergeCells count="9">
+    <mergeCell ref="A1:Y1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="F2:Y2"/>
     <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:U3"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:Y3"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.39375" right="0.39375" top="0.659027777777778" bottom="0.659027777777778" header="0.39375" footer="0.39375"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Обычный"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Страница &amp;P</oddFooter>

</xml_diff>